<commit_message>
Get 64-bit build working
</commit_message>
<xml_diff>
--- a/xllinet.xlsx
+++ b/xllinet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Inet</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>Return a range from a handle. Use cell menu 'Adjust' to get the entire range.</t>
+  </si>
+  <si>
+    <t>JSON.PARSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>JSON.VALUE</t>
+  </si>
+  <si>
+    <t>Get JSON data from a parsed object.</t>
+  </si>
+  <si>
+    <t>Get values from a JSON object using keys.</t>
   </si>
 </sst>
 </file>
@@ -393,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,12 +419,15 @@
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -417,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -425,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -433,20 +451,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>